<commit_message>
removing other as top genre
</commit_message>
<xml_diff>
--- a/Top_Artists.xlsx
+++ b/Top_Artists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnlam\Desktop\Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2880783F-9FE8-47A7-94D2-8EAC9304912E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDDADEE-1BC0-4005-9277-17451587B41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{46120A3A-E17E-42BB-BF78-D11EA92A16C5}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{46120A3A-E17E-42BB-BF78-D11EA92A16C5}"/>
   </bookViews>
   <sheets>
     <sheet name="X@Top10" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
-    <pivotCache cacheId="10" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -222,7 +222,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -379,49 +378,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1245,49 +1202,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3548,7 +3463,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5A30436-28CA-4978-AD42-76408D895EAD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5A30436-28CA-4978-AD42-76408D895EAD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -3687,7 +3602,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9646F5D4-2FEB-44DD-8FBB-CB1BEE75B102}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9646F5D4-2FEB-44DD-8FBB-CB1BEE75B102}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -4174,7 +4089,7 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>151.01</v>
       </c>
     </row>
@@ -4182,7 +4097,7 @@
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>151.01</v>
       </c>
     </row>
@@ -4190,7 +4105,7 @@
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>139</v>
       </c>
     </row>
@@ -4198,7 +4113,7 @@
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>139</v>
       </c>
     </row>
@@ -4206,7 +4121,7 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>5</v>
       </c>
     </row>
@@ -4214,7 +4129,7 @@
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>5</v>
       </c>
     </row>
@@ -4222,7 +4137,7 @@
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>295.01</v>
       </c>
     </row>
@@ -4236,7 +4151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8862C88-0884-4729-B335-2F3A79DE0F7F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4258,7 +4173,7 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>376965422</v>
       </c>
     </row>
@@ -4266,15 +4181,15 @@
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>376965422</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>376965422</v>
       </c>
     </row>
@@ -4282,7 +4197,7 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>534994242</v>
       </c>
     </row>
@@ -4290,15 +4205,15 @@
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>534994242</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>534994242</v>
       </c>
     </row>
@@ -4306,7 +4221,7 @@
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>263375966</v>
       </c>
     </row>
@@ -4314,15 +4229,15 @@
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>263375966</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>263375966</v>
       </c>
     </row>
@@ -4330,7 +4245,7 @@
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>1175335630</v>
       </c>
     </row>
@@ -4344,8 +4259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDD2C42-C45D-42CF-B07C-E64211C33C5C}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="A1:J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4355,7 +4270,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>